<commit_message>
-Show or hide gradients with a bit at the end.
</commit_message>
<xml_diff>
--- a/Concept diagrams/DrawGradient.xlsx
+++ b/Concept diagrams/DrawGradient.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingCopies\1st\FinalProj\branches\NewMethodology\Concept diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F34D8BC-1D91-4E27-9519-672697301CBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66311E55-3FBD-44BD-8AF6-E86A334BBCD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="40">
   <si>
     <t>Gradient</t>
   </si>
@@ -49,9 +49,6 @@
     <t>,1</t>
   </si>
   <si>
-    <t>)</t>
-  </si>
-  <si>
     <t>,2</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>Gradient Height</t>
+  </si>
+  <si>
+    <t>,)</t>
   </si>
 </sst>
 </file>
@@ -527,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A69AA61-9F1A-400C-972A-7070EA555679}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,21 +546,22 @@
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5703125" customWidth="1"/>
+    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3)</f>
-        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31)</v>
+        <f>_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3)</f>
+        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31,1,)</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -569,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -591,16 +592,22 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A34" si="0">_xlfn.CONCAT(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4)</f>
-        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30)</v>
+        <f t="shared" ref="A4:A34" si="0">_xlfn.CONCAT(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4)</f>
+        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30,1,)</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -609,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -632,16 +639,22 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29)</v>
+        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29,1,)</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -650,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -673,16 +686,22 @@
         <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28)</v>
+        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28,1,)</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -691,7 +710,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
@@ -714,16 +733,22 @@
         <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27)</v>
+        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27,1,)</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -732,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -755,16 +780,22 @@
         <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26)</v>
+        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26,1,)</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -773,7 +804,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -796,16 +827,22 @@
         <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25)</v>
+        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25,1,)</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -814,7 +851,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -837,16 +874,22 @@
         <v>28</v>
       </c>
       <c r="K9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24)</v>
+        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24,1,)</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -855,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -878,16 +921,22 @@
         <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23)</v>
+        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23,1,)</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -896,7 +945,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -919,16 +968,22 @@
         <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22)</v>
+        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22,1,)</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -937,7 +992,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -960,16 +1015,22 @@
         <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21)</v>
+        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21,1,)</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -978,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -1001,16 +1062,22 @@
         <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20)</v>
+        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20,1,)</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1019,7 +1086,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -1042,16 +1109,22 @@
         <v>48</v>
       </c>
       <c r="K14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19)</v>
+        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19,1,)</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1060,7 +1133,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -1083,16 +1156,22 @@
         <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18)</v>
+        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18,1,)</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -1101,7 +1180,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -1124,16 +1203,22 @@
         <v>56</v>
       </c>
       <c r="K16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17)</v>
+        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17,1,)</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1142,7 +1227,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
@@ -1165,16 +1250,22 @@
         <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16)</v>
+        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16,1,)</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -1183,7 +1274,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
@@ -1206,16 +1297,22 @@
         <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15)</v>
+        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15,1,)</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -1224,7 +1321,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -1247,16 +1344,22 @@
         <v>68</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14)</v>
+        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14,1,)</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -1265,7 +1368,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -1288,16 +1391,22 @@
         <v>72</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13)</v>
+        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13,1,)</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -1306,7 +1415,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -1329,16 +1438,22 @@
         <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12)</v>
+        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12,1,)</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -1347,7 +1462,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -1370,16 +1485,22 @@
         <v>80</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11)</v>
+        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11,1,)</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1388,7 +1509,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -1411,16 +1532,22 @@
         <v>84</v>
       </c>
       <c r="K23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10)</v>
+        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10,1,)</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1429,7 +1556,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
@@ -1452,16 +1579,22 @@
         <v>88</v>
       </c>
       <c r="K24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9)</v>
+        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9,1,)</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -1470,7 +1603,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -1493,16 +1626,22 @@
         <v>92</v>
       </c>
       <c r="K25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8)</v>
+        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8,1,)</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1511,7 +1650,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -1534,16 +1673,22 @@
         <v>96</v>
       </c>
       <c r="K26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7)</v>
+        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7,1,)</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -1552,7 +1697,7 @@
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
@@ -1575,16 +1720,22 @@
         <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6)</v>
+        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6,1,)</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -1593,7 +1744,7 @@
         <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
@@ -1616,16 +1767,22 @@
         <v>104</v>
       </c>
       <c r="K28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5)</v>
+        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5,1,)</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -1634,7 +1791,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
@@ -1657,16 +1814,22 @@
         <v>108</v>
       </c>
       <c r="K29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4)</v>
+        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4,1,)</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -1675,7 +1838,7 @@
         <v>27</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
@@ -1698,16 +1861,22 @@
         <v>112</v>
       </c>
       <c r="K30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3)</v>
+        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3,1,)</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -1716,7 +1885,7 @@
         <v>28</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
@@ -1739,16 +1908,22 @@
         <v>116</v>
       </c>
       <c r="K31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2)</v>
+        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2,1,)</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -1757,7 +1932,7 @@
         <v>29</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
@@ -1780,16 +1955,22 @@
         <v>120</v>
       </c>
       <c r="K32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1)</v>
+        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1,1,)</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -1798,7 +1979,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
@@ -1824,13 +2005,19 @@
         <v>4</v>
       </c>
       <c r="L33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0)</v>
+        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0,1,)</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
@@ -1839,7 +2026,7 @@
         <v>31</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
@@ -1862,13 +2049,19 @@
         <v>128</v>
       </c>
       <c r="K34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
   </sheetData>
@@ -1902,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,7 +2125,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,7 +2155,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,7 +2170,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1992,7 +2185,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2007,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,7 +2215,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2037,7 +2230,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2052,7 +2245,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,7 +2260,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,7 +2275,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,7 +2290,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,7 +2305,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,7 +2320,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2335,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2157,7 +2350,7 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,7 +2365,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2187,7 +2380,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2202,7 +2395,7 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,7 +2410,7 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,7 +2425,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2247,7 +2440,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2262,7 +2455,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,7 +2470,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2292,7 +2485,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,7 +2500,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2322,7 +2515,7 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2337,7 +2530,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,7 +2545,7 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2367,7 +2560,7 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-TO DO: Created a comment with a web link on how create list of objects and change attributes.
</commit_message>
<xml_diff>
--- a/Concept diagrams/DrawGradient.xlsx
+++ b/Concept diagrams/DrawGradient.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingCopies\1st\FinalProj\branches\NewMethodology\Concept diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66311E55-3FBD-44BD-8AF6-E86A334BBCD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310792B0-549C-4EB1-A07F-EC635FECB744}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <t>Gradient Height</t>
   </si>
   <si>
-    <t>,)</t>
+    <t>)</t>
   </si>
 </sst>
 </file>
@@ -529,9 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A69AA61-9F1A-400C-972A-7070EA555679}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -561,7 +559,7 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3)</f>
-        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31,1,)</v>
+        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31,1)</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -607,7 +605,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A34" si="0">_xlfn.CONCAT(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4)</f>
-        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30,1,)</v>
+        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30,1)</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -654,7 +652,7 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29,1,)</v>
+        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29,1)</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -701,7 +699,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28,1,)</v>
+        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28,1)</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -748,7 +746,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27,1,)</v>
+        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27,1)</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -795,7 +793,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26,1,)</v>
+        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26,1)</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -842,7 +840,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25,1,)</v>
+        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25,1)</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -889,7 +887,7 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24,1,)</v>
+        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24,1)</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -936,7 +934,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23,1,)</v>
+        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23,1)</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -983,7 +981,7 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22,1,)</v>
+        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22,1)</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -1030,7 +1028,7 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21,1,)</v>
+        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21,1)</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1077,7 +1075,7 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20,1,)</v>
+        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20,1)</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1124,7 +1122,7 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19,1,)</v>
+        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19,1)</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1171,7 +1169,7 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18,1,)</v>
+        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18,1)</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -1218,7 +1216,7 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17,1,)</v>
+        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17,1)</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1265,7 +1263,7 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16,1,)</v>
+        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16,1)</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -1312,7 +1310,7 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15,1,)</v>
+        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15,1)</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -1359,7 +1357,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14,1,)</v>
+        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14,1)</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -1406,7 +1404,7 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13,1,)</v>
+        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13,1)</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -1453,7 +1451,7 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12,1,)</v>
+        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12,1)</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -1500,7 +1498,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11,1,)</v>
+        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11,1)</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1547,7 +1545,7 @@
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10,1,)</v>
+        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10,1)</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1594,7 +1592,7 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9,1,)</v>
+        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9,1)</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -1641,7 +1639,7 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8,1,)</v>
+        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8,1)</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1688,7 +1686,7 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7,1,)</v>
+        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7,1)</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -1735,7 +1733,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6,1,)</v>
+        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6,1)</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -1782,7 +1780,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5,1,)</v>
+        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5,1)</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -1829,7 +1827,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4,1,)</v>
+        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4,1)</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -1876,7 +1874,7 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3,1,)</v>
+        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3,1)</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -1923,7 +1921,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2,1,)</v>
+        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2,1)</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -1970,7 +1968,7 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1,1,)</v>
+        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1,1)</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -2017,7 +2015,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0,1,)</v>
+        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0,1)</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
-Objects now have their own attributes.
</commit_message>
<xml_diff>
--- a/Concept diagrams/DrawGradient.xlsx
+++ b/Concept diagrams/DrawGradient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingCopies\1st\FinalProj\branches\NewMethodology\Concept diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310792B0-549C-4EB1-A07F-EC635FECB744}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE0B1A2-FE55-47A0-86EC-FB5AB24DE63F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
   </bookViews>
   <sheets>
     <sheet name="Gradients" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="40">
   <si>
     <t>Gradient</t>
   </si>
@@ -527,9 +527,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A69AA61-9F1A-400C-972A-7070EA555679}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -548,7 +550,7 @@
     <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -556,10 +558,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3)</f>
-        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31,1)</v>
+        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31)</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -593,19 +595,13 @@
         <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A34" si="0">_xlfn.CONCAT(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4)</f>
-        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30,1)</v>
+        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30)</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -640,19 +636,13 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29,1)</v>
+        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29)</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -687,19 +677,13 @@
         <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28,1)</v>
+        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28)</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -734,19 +718,13 @@
         <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27,1)</v>
+        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27)</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -781,19 +759,13 @@
         <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26,1)</v>
+        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26)</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -828,19 +800,13 @@
         <v>29</v>
       </c>
       <c r="L8" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25,1)</v>
+        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25)</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -875,19 +841,13 @@
         <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24,1)</v>
+        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24)</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -922,19 +882,13 @@
         <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23,1)</v>
+        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23)</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -969,19 +923,13 @@
         <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22,1)</v>
+        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22)</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -1016,19 +964,13 @@
         <v>25</v>
       </c>
       <c r="L12" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21,1)</v>
+        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21)</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1063,19 +1005,13 @@
         <v>24</v>
       </c>
       <c r="L13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20,1)</v>
+        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20)</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1110,19 +1046,13 @@
         <v>23</v>
       </c>
       <c r="L14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19,1)</v>
+        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19)</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1157,19 +1087,13 @@
         <v>22</v>
       </c>
       <c r="L15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18,1)</v>
+        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18)</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -1204,19 +1128,13 @@
         <v>21</v>
       </c>
       <c r="L16" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17,1)</v>
+        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17)</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1251,19 +1169,13 @@
         <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16,1)</v>
+        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16)</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -1298,19 +1210,13 @@
         <v>19</v>
       </c>
       <c r="L18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15,1)</v>
+        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15)</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -1345,19 +1251,13 @@
         <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14,1)</v>
+        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14)</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -1392,19 +1292,13 @@
         <v>17</v>
       </c>
       <c r="L20" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13,1)</v>
+        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13)</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -1439,19 +1333,13 @@
         <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12,1)</v>
+        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12)</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -1486,19 +1374,13 @@
         <v>15</v>
       </c>
       <c r="L22" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11,1)</v>
+        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11)</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1533,19 +1415,13 @@
         <v>14</v>
       </c>
       <c r="L23" t="s">
-        <v>2</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10,1)</v>
+        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10)</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1580,19 +1456,13 @@
         <v>13</v>
       </c>
       <c r="L24" t="s">
-        <v>2</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9,1)</v>
+        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9)</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -1627,19 +1497,13 @@
         <v>12</v>
       </c>
       <c r="L25" t="s">
-        <v>2</v>
-      </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8,1)</v>
+        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8)</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1674,19 +1538,13 @@
         <v>11</v>
       </c>
       <c r="L26" t="s">
-        <v>2</v>
-      </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7,1)</v>
+        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7)</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -1721,19 +1579,13 @@
         <v>10</v>
       </c>
       <c r="L27" t="s">
-        <v>2</v>
-      </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6,1)</v>
+        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6)</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -1768,19 +1620,13 @@
         <v>9</v>
       </c>
       <c r="L28" t="s">
-        <v>2</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5,1)</v>
+        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5)</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -1815,19 +1661,13 @@
         <v>8</v>
       </c>
       <c r="L29" t="s">
-        <v>2</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4,1)</v>
+        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4)</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -1862,19 +1702,13 @@
         <v>7</v>
       </c>
       <c r="L30" t="s">
-        <v>2</v>
-      </c>
-      <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3,1)</v>
+        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3)</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -1909,19 +1743,13 @@
         <v>6</v>
       </c>
       <c r="L31" t="s">
-        <v>2</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
-      </c>
-      <c r="N31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2,1)</v>
+        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2)</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -1956,19 +1784,13 @@
         <v>5</v>
       </c>
       <c r="L32" t="s">
-        <v>2</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1,1)</v>
+        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1)</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -2003,19 +1825,13 @@
         <v>4</v>
       </c>
       <c r="L33" t="s">
-        <v>2</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0,1)</v>
+        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0)</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
@@ -2050,16 +1866,10 @@
         <v>35</v>
       </c>
       <c r="L34" t="s">
-        <v>2</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
   </sheetData>
@@ -2071,7 +1881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901400BD-B244-43C7-AD79-1043749A3062}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
-Gradients can now be hidden
</commit_message>
<xml_diff>
--- a/Concept diagrams/DrawGradient.xlsx
+++ b/Concept diagrams/DrawGradient.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingCopies\1st\FinalProj\branches\NewMethodology\Concept diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE0B1A2-FE55-47A0-86EC-FB5AB24DE63F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF12F6-D1AA-4ADF-AB61-3605541F127B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="2" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
   </bookViews>
   <sheets>
     <sheet name="Gradients" sheetId="1" r:id="rId1"/>
     <sheet name="Draw" sheetId="2" r:id="rId2"/>
+    <sheet name="ChangeVisibility" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="41">
   <si>
     <t>Gradient</t>
   </si>
@@ -152,6 +153,9 @@
   </si>
   <si>
     <t>)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.IsObjectHidden = </t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901400BD-B244-43C7-AD79-1043749A3062}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2374,4 +2380,633 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4CA848-6235-4C95-B0D1-E897772A9C75}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>_xlfn.CONCAT(B1,C1,D1,E1)</f>
+        <v>Gradient0.IsObjectHidden = 0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A32" si="0">_xlfn.CONCAT(B2,C2,D2,E2)</f>
+        <v>Gradient1.IsObjectHidden = 0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <f>E1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient2.IsObjectHidden = 0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E32" si="1">E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient3.IsObjectHidden = 0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient4.IsObjectHidden = 0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient5.IsObjectHidden = 0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient6.IsObjectHidden = 0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient7.IsObjectHidden = 0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient8.IsObjectHidden = 0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient9.IsObjectHidden = 0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient10.IsObjectHidden = 0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient11.IsObjectHidden = 0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient12.IsObjectHidden = 0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient13.IsObjectHidden = 0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient14.IsObjectHidden = 0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient15.IsObjectHidden = 0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient16.IsObjectHidden = 0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient17.IsObjectHidden = 0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient18.IsObjectHidden = 0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient19.IsObjectHidden = 0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient20.IsObjectHidden = 0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient21.IsObjectHidden = 0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient22.IsObjectHidden = 0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient23.IsObjectHidden = 0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient24.IsObjectHidden = 0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient25.IsObjectHidden = 0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient26.IsObjectHidden = 0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient27.IsObjectHidden = 0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient28.IsObjectHidden = 0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient29.IsObjectHidden = 0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient30.IsObjectHidden = 0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>Gradient31.IsObjectHidden = 0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Objects are now in a list.
</commit_message>
<xml_diff>
--- a/Concept diagrams/DrawGradient.xlsx
+++ b/Concept diagrams/DrawGradient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingCopies\1st\FinalProj\branches\NewMethodology\Concept diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF12F6-D1AA-4ADF-AB61-3605541F127B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73050A06-37A5-4228-93D6-54D6780A7D70}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="2" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{49A42381-F339-4524-BD3A-55B3F16F8F22}"/>
   </bookViews>
   <sheets>
     <sheet name="Gradients" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="42">
   <si>
     <t>Gradient</t>
   </si>
@@ -143,19 +143,22 @@
     <t>,0</t>
   </si>
   <si>
-    <t>.draw()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> = Gradient (</t>
-  </si>
-  <si>
     <t>Gradient Height</t>
   </si>
   <si>
-    <t>)</t>
-  </si>
-  <si>
     <t xml:space="preserve">.IsObjectHidden = </t>
+  </si>
+  <si>
+    <t>.draw(canvas)</t>
+  </si>
+  <si>
+    <t>GradientList.append(</t>
+  </si>
+  <si>
+    <t>))</t>
+  </si>
+  <si>
+    <t>(</t>
   </si>
 </sst>
 </file>
@@ -531,1350 +534,1383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A69AA61-9F1A-400C-972A-7070EA555679}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.5703125" customWidth="1"/>
-    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" customWidth="1"/>
+    <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="3">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3)</f>
-        <v>Gradient0 = Gradient (canvas,0,0,xWidth,4,31)</v>
+        <f>_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3)</f>
+        <v>GradientList.append(Gradient(canvas,0,0,xWidth,4,31))</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <f>$B$1</f>
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <f>$C$1</f>
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>34</v>
       </c>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A34" si="0">_xlfn.CONCAT(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4)</f>
-        <v>Gradient1 = Gradient (canvas,0,4,xWidth,8,30)</v>
+        <f t="shared" ref="A4:A34" si="0">_xlfn.CONCAT(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4,O4)</f>
+        <v>GradientList.append(Gradient(canvas,0,4,xWidth,8,30))</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <f>H3+$B$1</f>
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f>I3+$C$1</f>
         <v>4</v>
       </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <f>J3+$B$1</f>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>K3+$C$1</f>
         <v>8</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>33</v>
       </c>
-      <c r="L4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="str">
+        <f>M3</f>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient2 = Gradient (canvas,0,8,xWidth,12,29)</v>
+        <v>GradientList.append(Gradient(canvas,0,8,xWidth,12,29))</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H34" si="1">H4+$B$1</f>
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I34" si="1">I4+$C$1</f>
         <v>8</v>
       </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J34" si="2">J4+$B$1</f>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K34" si="2">K4+$C$1</f>
         <v>12</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="str">
+        <f t="shared" ref="M5:M34" si="3">M4</f>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient3 = Gradient (canvas,0,12,xWidth,16,28)</v>
+        <v>GradientList.append(Gradient(canvas,0,12,xWidth,16,28))</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6">
+      <c r="J6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>31</v>
       </c>
-      <c r="L6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient4 = Gradient (canvas,0,16,xWidth,20,27)</v>
+        <v>GradientList.append(Gradient(canvas,0,16,xWidth,20,27))</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7">
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>30</v>
       </c>
-      <c r="L7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient5 = Gradient (canvas,0,20,xWidth,24,26)</v>
+        <v>GradientList.append(Gradient(canvas,0,20,xWidth,24,26))</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8">
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>29</v>
       </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient6 = Gradient (canvas,0,24,xWidth,28,25)</v>
+        <v>GradientList.append(Gradient(canvas,0,24,xWidth,28,25))</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9">
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient7 = Gradient (canvas,0,28,xWidth,32,24)</v>
+        <v>GradientList.append(Gradient(canvas,0,28,xWidth,32,24))</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10">
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>27</v>
       </c>
-      <c r="L10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient8 = Gradient (canvas,0,32,xWidth,36,23)</v>
+        <v>GradientList.append(Gradient(canvas,0,32,xWidth,36,23))</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11">
+      <c r="J11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>26</v>
       </c>
-      <c r="L11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient9 = Gradient (canvas,0,36,xWidth,40,22)</v>
+        <v>GradientList.append(Gradient(canvas,0,36,xWidth,40,22))</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12">
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient10 = Gradient (canvas,0,40,xWidth,44,21)</v>
+        <v>GradientList.append(Gradient(canvas,0,40,xWidth,44,21))</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13">
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>24</v>
       </c>
-      <c r="L13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient11 = Gradient (canvas,0,44,xWidth,48,20)</v>
+        <v>GradientList.append(Gradient(canvas,0,44,xWidth,48,20))</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14">
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="L14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient12 = Gradient (canvas,0,48,xWidth,52,19)</v>
+        <v>GradientList.append(Gradient(canvas,0,48,xWidth,52,19))</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15">
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>22</v>
       </c>
-      <c r="L15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient13 = Gradient (canvas,0,52,xWidth,56,18)</v>
+        <v>GradientList.append(Gradient(canvas,0,52,xWidth,56,18))</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="I16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16">
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>21</v>
       </c>
-      <c r="L16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient14 = Gradient (canvas,0,56,xWidth,60,17)</v>
+        <v>GradientList.append(Gradient(canvas,0,56,xWidth,60,17))</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="I17" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17">
+      <c r="J17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>20</v>
       </c>
-      <c r="L17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient15 = Gradient (canvas,0,60,xWidth,64,16)</v>
+        <v>GradientList.append(Gradient(canvas,0,60,xWidth,64,16))</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="I18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18">
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>19</v>
       </c>
-      <c r="L18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient16 = Gradient (canvas,0,64,xWidth,68,15)</v>
+        <v>GradientList.append(Gradient(canvas,0,64,xWidth,68,15))</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="I19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19">
+      <c r="J19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>18</v>
       </c>
-      <c r="L19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient17 = Gradient (canvas,0,68,xWidth,72,14)</v>
+        <v>GradientList.append(Gradient(canvas,0,68,xWidth,72,14))</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="I20" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20">
+      <c r="J20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>17</v>
       </c>
-      <c r="L20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient18 = Gradient (canvas,0,72,xWidth,76,13)</v>
+        <v>GradientList.append(Gradient(canvas,0,72,xWidth,76,13))</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>18</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="I21" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21">
+      <c r="J21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>16</v>
       </c>
-      <c r="L21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient19 = Gradient (canvas,0,76,xWidth,80,12)</v>
+        <v>GradientList.append(Gradient(canvas,0,76,xWidth,80,12))</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>19</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="I22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22">
+      <c r="J22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>15</v>
       </c>
-      <c r="L22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient20 = Gradient (canvas,0,80,xWidth,84,11)</v>
+        <v>GradientList.append(Gradient(canvas,0,80,xWidth,84,11))</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>20</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="I23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23">
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>14</v>
       </c>
-      <c r="L23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient21 = Gradient (canvas,0,84,xWidth,88,10)</v>
+        <v>GradientList.append(Gradient(canvas,0,84,xWidth,88,10))</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>21</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="I24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24">
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>13</v>
       </c>
-      <c r="L24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient22 = Gradient (canvas,0,88,xWidth,92,9)</v>
+        <v>GradientList.append(Gradient(canvas,0,88,xWidth,92,9))</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>22</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="I25" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25">
+      <c r="J25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>12</v>
       </c>
-      <c r="L25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient23 = Gradient (canvas,0,92,xWidth,96,8)</v>
+        <v>GradientList.append(Gradient(canvas,0,92,xWidth,96,8))</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>23</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="I26" t="s">
-        <v>3</v>
-      </c>
-      <c r="J26">
+      <c r="J26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>11</v>
       </c>
-      <c r="L26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient24 = Gradient (canvas,0,96,xWidth,100,7)</v>
+        <v>GradientList.append(Gradient(canvas,0,96,xWidth,100,7))</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>24</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="I27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27">
+      <c r="J27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>10</v>
       </c>
-      <c r="L27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient25 = Gradient (canvas,0,100,xWidth,104,6)</v>
+        <v>GradientList.append(Gradient(canvas,0,100,xWidth,104,6))</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>25</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="I28" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28">
+      <c r="J28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="2"/>
         <v>104</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>9</v>
       </c>
-      <c r="L28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient26 = Gradient (canvas,0,104,xWidth,108,5)</v>
+        <v>GradientList.append(Gradient(canvas,0,104,xWidth,108,5))</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>26</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="I29" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29">
+      <c r="J29" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>8</v>
       </c>
-      <c r="L29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient27 = Gradient (canvas,0,108,xWidth,112,4)</v>
+        <v>GradientList.append(Gradient(canvas,0,108,xWidth,112,4))</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>27</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="I30" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30">
+      <c r="J30" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="2"/>
         <v>112</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>7</v>
       </c>
-      <c r="L30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient28 = Gradient (canvas,0,112,xWidth,116,3)</v>
+        <v>GradientList.append(Gradient(canvas,0,112,xWidth,116,3))</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>28</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
-      </c>
-      <c r="H31">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="I31" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31">
+      <c r="J31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>6</v>
       </c>
-      <c r="L31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient29 = Gradient (canvas,0,116,xWidth,120,2)</v>
+        <v>GradientList.append(Gradient(canvas,0,116,xWidth,120,2))</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>29</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="I32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32">
+      <c r="J32" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>5</v>
       </c>
-      <c r="L32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient30 = Gradient (canvas,0,120,xWidth,124,1)</v>
+        <v>GradientList.append(Gradient(canvas,0,120,xWidth,124,1))</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>30</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="I33" t="s">
-        <v>3</v>
-      </c>
-      <c r="J33">
+      <c r="J33" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>4</v>
       </c>
-      <c r="L33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient31 = Gradient (canvas,0,124,xWidth,128,0)</v>
+        <v>GradientList.append(Gradient(canvas,0,124,xWidth,128,0))</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>31</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="I34" t="s">
-        <v>3</v>
-      </c>
-      <c r="J34">
+      <c r="J34" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>35</v>
       </c>
-      <c r="L34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="1"/>
+      <c r="M34" t="str">
+        <f t="shared" si="3"/>
+        <v>))</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1885,13 +1921,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901400BD-B244-43C7-AD79-1043749A3062}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -1900,7 +1934,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT(B1,C1,D1)</f>
-        <v>Gradient0.draw()</v>
+        <v>Gradient0.draw(canvas)</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1909,13 +1943,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A32" si="0">_xlfn.CONCAT(B2,C2,D2)</f>
-        <v>Gradient1.draw()</v>
+        <v>Gradient1.draw(canvas)</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1923,14 +1957,15 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
+      <c r="D2" t="str">
+        <f>D1</f>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient2.draw()</v>
+        <v>Gradient2.draw(canvas)</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1938,14 +1973,15 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D32" si="1">D2</f>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient3.draw()</v>
+        <v>Gradient3.draw(canvas)</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1953,14 +1989,15 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient4.draw()</v>
+        <v>Gradient4.draw(canvas)</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1968,14 +2005,15 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient5.draw()</v>
+        <v>Gradient5.draw(canvas)</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -1983,14 +2021,15 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>36</v>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient6.draw()</v>
+        <v>Gradient6.draw(canvas)</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -1998,14 +2037,15 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>36</v>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient7.draw()</v>
+        <v>Gradient7.draw(canvas)</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -2013,14 +2053,15 @@
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
-        <v>36</v>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient8.draw()</v>
+        <v>Gradient8.draw(canvas)</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -2028,14 +2069,15 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient9.draw()</v>
+        <v>Gradient9.draw(canvas)</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -2043,14 +2085,15 @@
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
-        <v>36</v>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient10.draw()</v>
+        <v>Gradient10.draw(canvas)</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -2058,14 +2101,15 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
-        <v>36</v>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient11.draw()</v>
+        <v>Gradient11.draw(canvas)</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -2073,14 +2117,15 @@
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient12.draw()</v>
+        <v>Gradient12.draw(canvas)</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -2088,14 +2133,15 @@
       <c r="C13">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
-        <v>36</v>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient13.draw()</v>
+        <v>Gradient13.draw(canvas)</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -2103,14 +2149,15 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
-        <v>36</v>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient14.draw()</v>
+        <v>Gradient14.draw(canvas)</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -2118,14 +2165,15 @@
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
-        <v>36</v>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient15.draw()</v>
+        <v>Gradient15.draw(canvas)</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -2133,14 +2181,15 @@
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
-        <v>36</v>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient16.draw()</v>
+        <v>Gradient16.draw(canvas)</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -2148,14 +2197,15 @@
       <c r="C17">
         <v>16</v>
       </c>
-      <c r="D17" t="s">
-        <v>36</v>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient17.draw()</v>
+        <v>Gradient17.draw(canvas)</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -2163,14 +2213,15 @@
       <c r="C18">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
-        <v>36</v>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient18.draw()</v>
+        <v>Gradient18.draw(canvas)</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -2178,14 +2229,15 @@
       <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
-        <v>36</v>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient19.draw()</v>
+        <v>Gradient19.draw(canvas)</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -2193,14 +2245,15 @@
       <c r="C20">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
-        <v>36</v>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient20.draw()</v>
+        <v>Gradient20.draw(canvas)</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -2208,14 +2261,15 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
-        <v>36</v>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient21.draw()</v>
+        <v>Gradient21.draw(canvas)</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -2223,14 +2277,15 @@
       <c r="C22">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
-        <v>36</v>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient22.draw()</v>
+        <v>Gradient22.draw(canvas)</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -2238,14 +2293,15 @@
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
-        <v>36</v>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient23.draw()</v>
+        <v>Gradient23.draw(canvas)</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -2253,14 +2309,15 @@
       <c r="C24">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
-        <v>36</v>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient24.draw()</v>
+        <v>Gradient24.draw(canvas)</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -2268,14 +2325,15 @@
       <c r="C25">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
-        <v>36</v>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient25.draw()</v>
+        <v>Gradient25.draw(canvas)</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -2283,14 +2341,15 @@
       <c r="C26">
         <v>25</v>
       </c>
-      <c r="D26" t="s">
-        <v>36</v>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient26.draw()</v>
+        <v>Gradient26.draw(canvas)</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -2298,14 +2357,15 @@
       <c r="C27">
         <v>26</v>
       </c>
-      <c r="D27" t="s">
-        <v>36</v>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient27.draw()</v>
+        <v>Gradient27.draw(canvas)</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -2313,14 +2373,15 @@
       <c r="C28">
         <v>27</v>
       </c>
-      <c r="D28" t="s">
-        <v>36</v>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient28.draw()</v>
+        <v>Gradient28.draw(canvas)</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -2328,14 +2389,15 @@
       <c r="C29">
         <v>28</v>
       </c>
-      <c r="D29" t="s">
-        <v>36</v>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient29.draw()</v>
+        <v>Gradient29.draw(canvas)</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -2343,14 +2405,15 @@
       <c r="C30">
         <v>29</v>
       </c>
-      <c r="D30" t="s">
-        <v>36</v>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient30.draw()</v>
+        <v>Gradient30.draw(canvas)</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -2358,14 +2421,15 @@
       <c r="C31">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
-        <v>36</v>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient31.draw()</v>
+        <v>Gradient31.draw(canvas)</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -2373,8 +2437,9 @@
       <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32" t="s">
-        <v>36</v>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>.draw(canvas)</v>
       </c>
     </row>
   </sheetData>
@@ -2386,9 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4CA848-6235-4C95-B0D1-E897772A9C75}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2399,7 +2462,7 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT(B1,C1,D1,E1)</f>
-        <v>Gradient0.IsObjectHidden = 0</v>
+        <v>Gradient0.IsObjectHidden = 1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2408,16 +2471,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A32" si="0">_xlfn.CONCAT(B2,C2,D2,E2)</f>
-        <v>Gradient1.IsObjectHidden = 0</v>
+        <v>Gradient1.IsObjectHidden = 1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2426,17 +2489,17 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <f>E1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient2.IsObjectHidden = 0</v>
+        <v>Gradient2.IsObjectHidden = 1</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2445,17 +2508,17 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E32" si="1">E2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient3.IsObjectHidden = 0</v>
+        <v>Gradient3.IsObjectHidden = 1</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2464,17 +2527,17 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient4.IsObjectHidden = 0</v>
+        <v>Gradient4.IsObjectHidden = 1</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -2483,17 +2546,17 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient5.IsObjectHidden = 0</v>
+        <v>Gradient5.IsObjectHidden = 1</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -2502,17 +2565,17 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient6.IsObjectHidden = 0</v>
+        <v>Gradient6.IsObjectHidden = 1</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -2521,17 +2584,17 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient7.IsObjectHidden = 0</v>
+        <v>Gradient7.IsObjectHidden = 1</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -2540,17 +2603,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient8.IsObjectHidden = 0</v>
+        <v>Gradient8.IsObjectHidden = 1</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -2559,17 +2622,17 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient9.IsObjectHidden = 0</v>
+        <v>Gradient9.IsObjectHidden = 1</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -2578,17 +2641,17 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient10.IsObjectHidden = 0</v>
+        <v>Gradient10.IsObjectHidden = 1</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -2597,17 +2660,17 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient11.IsObjectHidden = 0</v>
+        <v>Gradient11.IsObjectHidden = 1</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -2616,17 +2679,17 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient12.IsObjectHidden = 0</v>
+        <v>Gradient12.IsObjectHidden = 1</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -2635,17 +2698,17 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient13.IsObjectHidden = 0</v>
+        <v>Gradient13.IsObjectHidden = 1</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -2654,17 +2717,17 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient14.IsObjectHidden = 0</v>
+        <v>Gradient14.IsObjectHidden = 1</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -2673,17 +2736,17 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient15.IsObjectHidden = 0</v>
+        <v>Gradient15.IsObjectHidden = 1</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -2692,17 +2755,17 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient16.IsObjectHidden = 0</v>
+        <v>Gradient16.IsObjectHidden = 1</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -2711,17 +2774,17 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient17.IsObjectHidden = 0</v>
+        <v>Gradient17.IsObjectHidden = 1</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -2730,17 +2793,17 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient18.IsObjectHidden = 0</v>
+        <v>Gradient18.IsObjectHidden = 1</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -2749,17 +2812,17 @@
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient19.IsObjectHidden = 0</v>
+        <v>Gradient19.IsObjectHidden = 1</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -2768,17 +2831,17 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient20.IsObjectHidden = 0</v>
+        <v>Gradient20.IsObjectHidden = 1</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -2787,17 +2850,17 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient21.IsObjectHidden = 0</v>
+        <v>Gradient21.IsObjectHidden = 1</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -2806,17 +2869,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient22.IsObjectHidden = 0</v>
+        <v>Gradient22.IsObjectHidden = 1</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -2825,17 +2888,17 @@
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient23.IsObjectHidden = 0</v>
+        <v>Gradient23.IsObjectHidden = 1</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -2844,17 +2907,17 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient24.IsObjectHidden = 0</v>
+        <v>Gradient24.IsObjectHidden = 1</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -2863,17 +2926,17 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient25.IsObjectHidden = 0</v>
+        <v>Gradient25.IsObjectHidden = 1</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -2882,17 +2945,17 @@
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient26.IsObjectHidden = 0</v>
+        <v>Gradient26.IsObjectHidden = 1</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -2901,17 +2964,17 @@
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient27.IsObjectHidden = 0</v>
+        <v>Gradient27.IsObjectHidden = 1</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -2920,17 +2983,17 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient28.IsObjectHidden = 0</v>
+        <v>Gradient28.IsObjectHidden = 1</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -2939,17 +3002,17 @@
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient29.IsObjectHidden = 0</v>
+        <v>Gradient29.IsObjectHidden = 1</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -2958,17 +3021,17 @@
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient30.IsObjectHidden = 0</v>
+        <v>Gradient30.IsObjectHidden = 1</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -2977,17 +3040,17 @@
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>Gradient31.IsObjectHidden = 0</v>
+        <v>Gradient31.IsObjectHidden = 1</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -2996,11 +3059,11 @@
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>